<commit_message>
Rename LED_1234 to LED_ABCD
</commit_message>
<xml_diff>
--- a/Documents/RP2040_PICO_pinout.xlsx
+++ b/Documents/RP2040_PICO_pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jth\Pico\jim_code\Robokid_Pico_FreeRTOS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A6F193-0EBA-471F-A757-E470EC7F1547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACC8C15-B3F4-463C-8A3A-E79FF3CFA7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{744D44B9-5EF3-4418-910E-104F8A1D63F4}"/>
+    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{744D44B9-5EF3-4418-910E-104F8A1D63F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="109">
   <si>
     <t>RP2040 chip pin</t>
   </si>
@@ -282,6 +282,84 @@
   </si>
   <si>
     <t>Production</t>
+  </si>
+  <si>
+    <t>(FTDI Vitrual Com Port TX)</t>
+  </si>
+  <si>
+    <t>(FTDI Vitrual Com Port RX)</t>
+  </si>
+  <si>
+    <t>Left motor control A</t>
+  </si>
+  <si>
+    <t>Left motor control B</t>
+  </si>
+  <si>
+    <t>Right motor control A</t>
+  </si>
+  <si>
+    <t>Right motor control B</t>
+  </si>
+  <si>
+    <t>Push button A</t>
+  </si>
+  <si>
+    <t>Push button B</t>
+  </si>
+  <si>
+    <t>Push button C</t>
+  </si>
+  <si>
+    <t>Push button D</t>
+  </si>
+  <si>
+    <t>LED A</t>
+  </si>
+  <si>
+    <t>LED B</t>
+  </si>
+  <si>
+    <t>LED C</t>
+  </si>
+  <si>
+    <t>LED D</t>
+  </si>
+  <si>
+    <t>Sounder</t>
+  </si>
+  <si>
+    <t>SSD1306 I2C SDA</t>
+  </si>
+  <si>
+    <t>SSD1306 I2C SCL</t>
+  </si>
+  <si>
+    <t>Analogue channel</t>
+  </si>
+  <si>
+    <t>(IR input)</t>
+  </si>
+  <si>
+    <t>(PICO LED)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>CD4051 feed</t>
+  </si>
+  <si>
+    <t>(Indicator 2 : Misc LED)</t>
+  </si>
+  <si>
+    <t>(Indicator 1 : USB LED)</t>
+  </si>
+  <si>
+    <t>FTDI  FT234XD</t>
   </si>
 </sst>
 </file>
@@ -310,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +398,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,12 +420,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -658,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19889A31-2C0F-4C84-B1B4-4FC1374F5BC2}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,11 +757,12 @@
     <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -693,8 +781,11 @@
       <c r="F1" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -702,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -715,8 +806,17 @@
       <c r="D3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -729,8 +829,17 @@
       <c r="D4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -744,7 +853,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -758,7 +867,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -771,8 +880,11 @@
       <c r="D7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -785,8 +897,11 @@
       <c r="D8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -799,8 +914,11 @@
       <c r="D9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -814,7 +932,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -822,7 +940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -835,8 +953,11 @@
       <c r="D12" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -849,8 +970,11 @@
       <c r="D13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -864,7 +988,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -877,8 +1001,14 @@
       <c r="D15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -891,8 +1021,11 @@
       <c r="D16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -905,8 +1038,11 @@
       <c r="D17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -919,8 +1055,11 @@
       <c r="D18" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -933,72 +1072,83 @@
       <c r="D19" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1011,8 +1161,11 @@
       <c r="D28" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1025,8 +1178,11 @@
       <c r="D29" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1039,8 +1195,11 @@
       <c r="D30" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1053,8 +1212,11 @@
       <c r="D31" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1067,8 +1229,11 @@
       <c r="D32" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1081,16 +1246,20 @@
       <c r="D33" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1104,23 +1273,25 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1131,10 +1302,10 @@
         <v>53</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1147,8 +1318,14 @@
       <c r="D39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1161,8 +1338,11 @@
       <c r="D40" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1175,134 +1355,153 @@
       <c r="D41" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="C57" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
config param to set push switch default
</commit_message>
<xml_diff>
--- a/Documents/RP2040_PICO_pinout.xlsx
+++ b/Documents/RP2040_PICO_pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jth\Pico\jim_code\Robokid_Pico_FreeRTOS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACC8C15-B3F4-463C-8A3A-E79FF3CFA7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA61DD9-7C07-495F-A950-268D116A96DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{744D44B9-5EF3-4418-910E-104F8A1D63F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{744D44B9-5EF3-4418-910E-104F8A1D63F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
   <si>
     <t>RP2040 chip pin</t>
   </si>
@@ -353,13 +353,13 @@
     <t>CD4051 feed</t>
   </si>
   <si>
-    <t>(Indicator 2 : Misc LED)</t>
-  </si>
-  <si>
-    <t>(Indicator 1 : USB LED)</t>
-  </si>
-  <si>
     <t>FTDI  FT234XD</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>CD4051  select A</t>
   </si>
 </sst>
 </file>
@@ -745,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19889A31-2C0F-4C84-B1B4-4FC1374F5BC2}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +762,7 @@
     <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -785,7 +785,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -793,7 +793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -813,10 +813,10 @@
         <v>83</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -836,10 +836,10 @@
         <v>84</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -852,8 +852,11 @@
       <c r="D5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -866,8 +869,11 @@
       <c r="D6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -881,10 +887,10 @@
         <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -898,10 +904,10 @@
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -914,11 +920,8 @@
       <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="E9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -932,7 +935,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -940,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -957,7 +960,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -974,7 +977,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -987,8 +990,11 @@
       <c r="D14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1008,7 +1014,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1505,7 +1511,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.39370078740157483" bottom="0.74803149606299213" header="0.39370078740157483" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lots of edits; added basic Neopixel code
</commit_message>
<xml_diff>
--- a/Documents/RP2040_PICO_pinout.xlsx
+++ b/Documents/RP2040_PICO_pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jth\Pico\jim_code\Robokid_Pico_FreeRTOS\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA61DD9-7C07-495F-A950-268D116A96DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09134C2C-3C71-4061-B1B3-ABFCEBA9E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{744D44B9-5EF3-4418-910E-104F8A1D63F4}"/>
   </bookViews>
@@ -314,18 +314,6 @@
     <t>Push button D</t>
   </si>
   <si>
-    <t>LED A</t>
-  </si>
-  <si>
-    <t>LED B</t>
-  </si>
-  <si>
-    <t>LED C</t>
-  </si>
-  <si>
-    <t>LED D</t>
-  </si>
-  <si>
     <t>Sounder</t>
   </si>
   <si>
@@ -360,13 +348,116 @@
   </si>
   <si>
     <t>CD4051  select A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LED B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LED C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LED D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LED A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Neopixel OUT</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,8 +478,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +514,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -420,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -429,6 +542,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -748,7 +864,7 @@
   <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,7 +898,7 @@
         <v>82</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -813,7 +929,7 @@
         <v>83</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -836,24 +952,24 @@
         <v>84</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -870,7 +986,7 @@
         <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -887,7 +1003,7 @@
         <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -904,17 +1020,17 @@
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>9</v>
       </c>
       <c r="D9" t="s">
@@ -925,10 +1041,10 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>10</v>
       </c>
       <c r="D10" t="s">
@@ -957,7 +1073,7 @@
         <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -974,7 +1090,7 @@
         <v>64</v>
       </c>
       <c r="E13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -991,7 +1107,7 @@
         <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1008,10 +1124,10 @@
         <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1168,24 +1284,24 @@
         <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="4">
         <v>22</v>
       </c>
       <c r="D29" t="s">
         <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1269,10 +1385,10 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="4">
         <v>29</v>
       </c>
       <c r="D35" t="s">
@@ -1308,7 +1424,7 @@
         <v>53</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1325,44 +1441,44 @@
         <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="4">
         <v>32</v>
       </c>
       <c r="D40" t="s">
         <v>78</v>
       </c>
       <c r="E40" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41" s="4">
         <v>34</v>
       </c>
       <c r="D41" t="s">
         <v>79</v>
       </c>
       <c r="E41" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>